<commit_message>
some style clear entries
</commit_message>
<xml_diff>
--- a/pythonProject/P2P_History_YesterdayBinance.xlsx
+++ b/pythonProject/P2P_History_YesterdayBinance.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:M40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -485,7 +485,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3999</v>
+        <v>1141</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -494,7 +494,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2024-06-09 21:40:15</t>
+          <t>2024-06-10 23:02:15</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
@@ -504,7 +504,7 @@
         </is>
       </c>
       <c r="I2" t="n">
-        <v>2700</v>
+        <v>2044</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -513,12 +513,12 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2024-06-09 23:24:54</t>
+          <t>2024-06-10 23:42:09</t>
         </is>
       </c>
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="n">
-        <v>-1101.349999999999</v>
+        <v>56872.89999999999</v>
       </c>
     </row>
     <row r="3">
@@ -528,7 +528,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1795</v>
+        <v>1094</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -537,7 +537,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2024-06-09 21:30:06</t>
+          <t>2024-06-10 22:52:38</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
@@ -547,7 +547,7 @@
         </is>
       </c>
       <c r="I3" t="n">
-        <v>4000</v>
+        <v>1200</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -556,7 +556,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2024-06-09 22:18:36</t>
+          <t>2024-06-10 23:38:53</t>
         </is>
       </c>
       <c r="L3" t="inlineStr"/>
@@ -568,7 +568,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1994</v>
+        <v>1595</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -577,17 +577,17 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2024-06-09 21:29:16</t>
+          <t>2024-06-10 22:37:07</t>
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
       <c r="H4" t="inlineStr">
         <is>
-          <t>CANCELLED</t>
+          <t>COMPLETED</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>1500</v>
+        <v>2023</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -596,7 +596,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2024-06-09 22:09:05</t>
+          <t>2024-06-10 23:19:51</t>
         </is>
       </c>
       <c r="L4" t="inlineStr"/>
@@ -604,11 +604,11 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>CANCELLED</t>
+          <t>COMPLETED</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1212</v>
+        <v>2953</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -617,17 +617,17 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2024-06-09 21:27:09</t>
+          <t>2024-06-10 14:40:03</t>
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
       <c r="H5" t="inlineStr">
         <is>
-          <t>COMPLETED</t>
+          <t>CANCELLED_BY_SYSTEM</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>1000</v>
+        <v>1200</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -636,7 +636,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2024-06-09 22:09:04</t>
+          <t>2024-06-10 23:17:06</t>
         </is>
       </c>
       <c r="L5" t="inlineStr"/>
@@ -648,7 +648,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>3185</v>
+        <v>3561</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -657,7 +657,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2024-06-09 21:02:34</t>
+          <t>2024-06-10 14:18:36</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
@@ -667,7 +667,7 @@
         </is>
       </c>
       <c r="I6" t="n">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -676,7 +676,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2024-06-09 22:04:16</t>
+          <t>2024-06-10 22:28:12</t>
         </is>
       </c>
       <c r="L6" t="inlineStr"/>
@@ -688,7 +688,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1994</v>
+        <v>1201</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -697,7 +697,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2024-06-09 19:44:19</t>
+          <t>2024-06-10 14:11:33</t>
         </is>
       </c>
       <c r="E7" t="inlineStr"/>
@@ -707,7 +707,7 @@
         </is>
       </c>
       <c r="I7" t="n">
-        <v>1000</v>
+        <v>3000</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -716,7 +716,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2024-06-09 21:56:16</t>
+          <t>2024-06-10 22:04:38</t>
         </is>
       </c>
       <c r="L7" t="inlineStr"/>
@@ -728,7 +728,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2645</v>
+        <v>2600</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -737,17 +737,17 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2024-06-09 19:38:02</t>
+          <t>2024-06-10 14:08:44</t>
         </is>
       </c>
       <c r="E8" t="inlineStr"/>
       <c r="H8" t="inlineStr">
         <is>
-          <t>CANCELLED</t>
+          <t>COMPLETED</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>2000</v>
+        <v>1500</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -756,7 +756,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>2024-06-09 21:55:29</t>
+          <t>2024-06-10 22:00:42</t>
         </is>
       </c>
       <c r="L8" t="inlineStr"/>
@@ -768,7 +768,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1436</v>
+        <v>2122</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -777,17 +777,17 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2024-06-09 18:32:53</t>
+          <t>2024-06-10 14:04:17</t>
         </is>
       </c>
       <c r="E9" t="inlineStr"/>
       <c r="H9" t="inlineStr">
         <is>
-          <t>CANCELLED</t>
+          <t>COMPLETED</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>4000</v>
+        <v>2510</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -796,7 +796,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2024-06-09 21:53:23</t>
+          <t>2024-06-10 21:50:16</t>
         </is>
       </c>
       <c r="L9" t="inlineStr"/>
@@ -808,7 +808,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1647</v>
+        <v>1343</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -817,7 +817,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2024-06-09 18:27:13</t>
+          <t>2024-06-10 13:57:07</t>
         </is>
       </c>
       <c r="E10" t="inlineStr"/>
@@ -827,7 +827,7 @@
         </is>
       </c>
       <c r="I10" t="n">
-        <v>1800</v>
+        <v>2500</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -836,38 +836,19 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>2024-06-09 21:47:51</t>
+          <t>2024-06-10 21:32:31</t>
         </is>
       </c>
       <c r="L10" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>COMPLETED</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>3790</v>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>BUY</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>2024-06-09 17:33:41</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr"/>
       <c r="H11" t="inlineStr">
         <is>
-          <t>COMPLETED</t>
+          <t>CANCELLED</t>
         </is>
       </c>
       <c r="I11" t="n">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -876,38 +857,19 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2024-06-09 21:43:51</t>
+          <t>2024-06-10 21:23:48</t>
         </is>
       </c>
       <c r="L11" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>COMPLETED</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>1998</v>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>BUY</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>2024-06-09 17:28:12</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr"/>
       <c r="H12" t="inlineStr">
         <is>
-          <t>CANCELLED</t>
+          <t>COMPLETED</t>
         </is>
       </c>
       <c r="I12" t="n">
-        <v>1600</v>
+        <v>2424</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -916,7 +878,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2024-06-09 21:43:39</t>
+          <t>2024-06-10 21:18:19</t>
         </is>
       </c>
       <c r="L12" t="inlineStr"/>
@@ -928,7 +890,7 @@
         </is>
       </c>
       <c r="I13" t="n">
-        <v>2000</v>
+        <v>1200</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -937,7 +899,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2024-06-09 21:39:40</t>
+          <t>2024-06-10 21:13:11</t>
         </is>
       </c>
       <c r="L13" t="inlineStr"/>
@@ -945,7 +907,7 @@
     <row r="14">
       <c r="H14" t="inlineStr">
         <is>
-          <t>CANCELLED</t>
+          <t>COMPLETED</t>
         </is>
       </c>
       <c r="I14" t="n">
@@ -958,10 +920,556 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>2024-06-09 20:24:11</t>
+          <t>2024-06-10 21:12:05</t>
         </is>
       </c>
       <c r="L14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>COMPLETED</t>
+        </is>
+      </c>
+      <c r="I15" t="n">
+        <v>1000</v>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>2024-06-10 21:11:46</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>CANCELLED_BY_SYSTEM</t>
+        </is>
+      </c>
+      <c r="I16" t="n">
+        <v>4000</v>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>2024-06-10 21:09:32</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>CANCELLED</t>
+        </is>
+      </c>
+      <c r="I17" t="n">
+        <v>1400</v>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>2024-06-10 21:02:49</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>COMPLETED</t>
+        </is>
+      </c>
+      <c r="I18" t="n">
+        <v>1900</v>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>2024-06-10 20:59:25</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>CANCELLED_BY_SYSTEM</t>
+        </is>
+      </c>
+      <c r="I19" t="n">
+        <v>1900</v>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>2024-06-10 20:51:19</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>CANCELLED</t>
+        </is>
+      </c>
+      <c r="I20" t="n">
+        <v>3600</v>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>2024-06-10 20:37:12</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>COMPLETED</t>
+        </is>
+      </c>
+      <c r="I21" t="n">
+        <v>1285</v>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>2024-06-10 19:37:29</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>CANCELLED</t>
+        </is>
+      </c>
+      <c r="I22" t="n">
+        <v>1000</v>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>2024-06-10 18:52:45</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>CANCELLED_BY_SYSTEM</t>
+        </is>
+      </c>
+      <c r="I23" t="n">
+        <v>4000</v>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>2024-06-10 18:46:44</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>CANCELLED</t>
+        </is>
+      </c>
+      <c r="I24" t="n">
+        <v>4000</v>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>2024-06-10 18:34:34</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>COMPLETED</t>
+        </is>
+      </c>
+      <c r="I25" t="n">
+        <v>4000</v>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>2024-06-10 16:12:40</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>CANCELLED</t>
+        </is>
+      </c>
+      <c r="I26" t="n">
+        <v>1700</v>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>2024-06-10 16:01:28</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>COMPLETED</t>
+        </is>
+      </c>
+      <c r="I27" t="n">
+        <v>2000</v>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>2024-06-10 15:28:06</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>COMPLETED</t>
+        </is>
+      </c>
+      <c r="I28" t="n">
+        <v>1000</v>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>2024-06-10 14:59:55</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>COMPLETED</t>
+        </is>
+      </c>
+      <c r="I29" t="n">
+        <v>1000</v>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>2024-06-10 14:48:36</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr"/>
+    </row>
+    <row r="30">
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>CANCELLED</t>
+        </is>
+      </c>
+      <c r="I30" t="n">
+        <v>1000</v>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>2024-06-10 14:45:30</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr"/>
+    </row>
+    <row r="31">
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>COMPLETED</t>
+        </is>
+      </c>
+      <c r="I31" t="n">
+        <v>1000</v>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>2024-06-10 14:33:36</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>COMPLETED</t>
+        </is>
+      </c>
+      <c r="I32" t="n">
+        <v>1000</v>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>2024-06-10 14:33:02</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr"/>
+    </row>
+    <row r="33">
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>COMPLETED</t>
+        </is>
+      </c>
+      <c r="I33" t="n">
+        <v>1600</v>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>2024-06-10 14:28:05</t>
+        </is>
+      </c>
+      <c r="L33" t="inlineStr"/>
+    </row>
+    <row r="34">
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>COMPLETED</t>
+        </is>
+      </c>
+      <c r="I34" t="n">
+        <v>1000</v>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>2024-06-10 14:23:16</t>
+        </is>
+      </c>
+      <c r="L34" t="inlineStr"/>
+    </row>
+    <row r="35">
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>CANCELLED_BY_SYSTEM</t>
+        </is>
+      </c>
+      <c r="I35" t="n">
+        <v>2000</v>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>2024-06-10 14:19:13</t>
+        </is>
+      </c>
+      <c r="L35" t="inlineStr"/>
+    </row>
+    <row r="36">
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>COMPLETED</t>
+        </is>
+      </c>
+      <c r="I36" t="n">
+        <v>1000</v>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>2024-06-10 14:12:30</t>
+        </is>
+      </c>
+      <c r="L36" t="inlineStr"/>
+    </row>
+    <row r="37">
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>CANCELLED</t>
+        </is>
+      </c>
+      <c r="I37" t="n">
+        <v>4000</v>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>2024-06-10 14:10:13</t>
+        </is>
+      </c>
+      <c r="L37" t="inlineStr"/>
+    </row>
+    <row r="38">
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>CANCELLED</t>
+        </is>
+      </c>
+      <c r="I38" t="n">
+        <v>1500</v>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>2024-06-10 13:53:30</t>
+        </is>
+      </c>
+      <c r="L38" t="inlineStr"/>
+    </row>
+    <row r="39">
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>COMPLETED</t>
+        </is>
+      </c>
+      <c r="I39" t="n">
+        <v>1000</v>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>2024-06-10 13:47:01</t>
+        </is>
+      </c>
+      <c r="L39" t="inlineStr"/>
+    </row>
+    <row r="40">
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>COMPLETED</t>
+        </is>
+      </c>
+      <c r="I40" t="n">
+        <v>1000</v>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>2024-06-10 13:44:55</t>
+        </is>
+      </c>
+      <c r="L40" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>